<commit_message>
updated master sheet, some fig edits, sess 2 & 3 data
I had the incorrect boxes marked in the master sheet, corrected those.

Added data from session 2 and 3. Corrected female filenames and "subject" data from sessions 0 and 1 because I had put the wrong subject labels in the macros.

Some edits to daily figures to avoid wonky results with scant data. Started editing publication figures likewise but not complete yet. will still error if run.
</commit_message>
<xml_diff>
--- a/Coffey R00 Master Key.xlsx
+++ b/Coffey R00 Master Key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schle\Documents\GitHub\CoffeyBehavior_RatEdition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A745C48-B680-4A05-B384-4449E21BA9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0107BC-52D7-43C0-946D-6D9D892D37EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="59">
   <si>
     <t>Tag Number</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>Afternoon</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>euthanized 3/24/25 (bad implant)</t>
+  </si>
+  <si>
+    <t>{0, 1}</t>
+  </si>
+  <si>
+    <t>{2}</t>
   </si>
 </sst>
 </file>
@@ -287,9 +299,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}" name="Table1" displayName="Table1" ref="A1:V48" totalsRowShown="0">
-  <autoFilter ref="A1:V48" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}" name="Table1" displayName="Table1" ref="A1:W48" totalsRowShown="0">
+  <autoFilter ref="A1:W48" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}"/>
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{60D7D7A6-CBAB-41C3-A922-12D9BB352B61}" name="Tag Number"/>
     <tableColumn id="10" xr3:uid="{CAA37174-1539-4368-836A-0F1CD6010E9C}" name="Run"/>
     <tableColumn id="2" xr3:uid="{AAA8256D-38B9-490E-86D1-0A386D831626}" name="Tag Color"/>
@@ -311,7 +323,8 @@
     <tableColumn id="18" xr3:uid="{567717B4-321E-4E6A-A33E-5FEB4544E2B6}" name="RemoveSession"/>
     <tableColumn id="11" xr3:uid="{0AFA8CA7-4137-4911-9BDA-2CA56DB483CB}" name="MedPC Data Folder"/>
     <tableColumn id="9" xr3:uid="{EE0658C2-4F47-4187-9F03-0604EA21891A}" name="USV Data Folder"/>
-    <tableColumn id="12" xr3:uid="{3692F92B-7339-4679-8FAA-0EBB775BF247}" name="Video Data Folder"/>
+    <tableColumn id="20" xr3:uid="{DA846ABF-3C4A-46BA-958E-0334DFCFCAEE}" name="Video Data Folder"/>
+    <tableColumn id="12" xr3:uid="{3692F92B-7339-4679-8FAA-0EBB775BF247}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -580,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,22 +605,25 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" customWidth="1"/>
     <col min="14" max="15" width="18.5703125" customWidth="1"/>
     <col min="16" max="16" width="16.7109375" customWidth="1"/>
     <col min="17" max="18" width="22.140625" customWidth="1"/>
-    <col min="19" max="20" width="122.5703125" customWidth="1"/>
-    <col min="21" max="21" width="135.5703125" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="21.5703125" customWidth="1"/>
+    <col min="21" max="21" width="23.7109375" customWidth="1"/>
+    <col min="22" max="22" width="25.5703125" customWidth="1"/>
+    <col min="23" max="23" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -674,8 +690,11 @@
       <c r="V1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>33</v>
       </c>
@@ -710,7 +729,7 @@
         <v>17</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N2" t="s">
         <v>53</v>
@@ -728,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>34</v>
       </c>
@@ -766,7 +785,7 @@
         <v>17</v>
       </c>
       <c r="M3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N3" t="s">
         <v>53</v>
@@ -787,7 +806,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>35</v>
       </c>
@@ -822,7 +841,7 @@
         <v>17</v>
       </c>
       <c r="M4">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N4" t="s">
         <v>53</v>
@@ -844,8 +863,9 @@
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>36</v>
       </c>
@@ -880,7 +900,7 @@
         <v>17</v>
       </c>
       <c r="M5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N5" t="s">
         <v>53</v>
@@ -901,7 +921,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>37</v>
       </c>
@@ -936,7 +956,7 @@
         <v>17</v>
       </c>
       <c r="M6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="N6" t="s">
         <v>53</v>
@@ -957,7 +977,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>38</v>
       </c>
@@ -992,7 +1012,7 @@
         <v>17</v>
       </c>
       <c r="M7">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="N7" t="s">
         <v>53</v>
@@ -1013,7 +1033,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>39</v>
       </c>
@@ -1048,7 +1068,7 @@
         <v>17</v>
       </c>
       <c r="M8">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="N8" t="s">
         <v>53</v>
@@ -1069,7 +1089,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>40</v>
       </c>
@@ -1104,7 +1124,7 @@
         <v>17</v>
       </c>
       <c r="M9">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N9" t="s">
         <v>53</v>
@@ -1122,10 +1142,13 @@
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="W9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>41</v>
       </c>
@@ -1160,7 +1183,7 @@
         <v>17</v>
       </c>
       <c r="M10">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N10" t="s">
         <v>54</v>
@@ -1181,7 +1204,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>42</v>
       </c>
@@ -1216,7 +1239,7 @@
         <v>17</v>
       </c>
       <c r="M11">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N11" t="s">
         <v>54</v>
@@ -1237,7 +1260,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>43</v>
       </c>
@@ -1272,7 +1295,7 @@
         <v>17</v>
       </c>
       <c r="M12">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="N12" t="s">
         <v>54</v>
@@ -1293,7 +1316,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>44</v>
       </c>
@@ -1328,7 +1351,7 @@
         <v>17</v>
       </c>
       <c r="M13">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N13" t="s">
         <v>54</v>
@@ -1349,7 +1372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>45</v>
       </c>
@@ -1384,7 +1407,7 @@
         <v>17</v>
       </c>
       <c r="M14">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="N14" t="s">
         <v>54</v>
@@ -1405,7 +1428,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>46</v>
       </c>
@@ -1440,7 +1463,7 @@
         <v>17</v>
       </c>
       <c r="M15">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="N15" t="s">
         <v>54</v>
@@ -1461,7 +1484,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>47</v>
       </c>
@@ -1496,7 +1519,7 @@
         <v>17</v>
       </c>
       <c r="M16">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="N16" t="s">
         <v>54</v>
@@ -1517,7 +1540,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>48</v>
       </c>
@@ -1552,7 +1575,7 @@
         <v>17</v>
       </c>
       <c r="M17">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="N17" t="s">
         <v>54</v>
@@ -1573,57 +1596,58 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F20" s="1"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>